<commit_message>
Maj + ajout mdp iddentifiant
</commit_message>
<xml_diff>
--- a/OPEN_sujet1_application/messages.xlsx
+++ b/OPEN_sujet1_application/messages.xlsx
@@ -1,80 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hadrien\ISARA\ISARA P4\OPEN\R_Module_1b\TD\OPEN_sujet1\OPEN_sujet1_application\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6608D7B-59EA-4505-AD01-5664B489AA91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
-  <si>
-    <t>Nom</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Message</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>schmitt</t>
-  </si>
-  <si>
-    <t>hschmitt@etu.isara.fr</t>
-  </si>
-  <si>
-    <t>testttt</t>
-  </si>
-  <si>
-    <t>hschmitt@etu.Isara.fr</t>
-  </si>
-  <si>
-    <t>testtt</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>hschmitt</t>
-  </si>
-  <si>
-    <t>APPLICATIONNN</t>
-  </si>
-  <si>
-    <t>hdhdhd</t>
-  </si>
-  <si>
-    <t>jhfhhfjdhdf</t>
-  </si>
-  <si>
-    <t>jhhfhehe</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss\ \U\T\C"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd HH:mm:ss UTC"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,21 +67,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -175,7 +111,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -209,7 +145,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -244,10 +179,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -420,100 +354,156 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nom</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Message</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>schmitt</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>hschmitt@etu.isara.fr</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>testttt</t>
+        </is>
       </c>
       <c r="D2" s="2">
         <v>45699.50648512732</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>schmitt</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>hschmitt@etu.Isara.fr</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>testtt</t>
+        </is>
       </c>
       <c r="D3" s="2">
-        <v>45699.506859340283</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
+        <v>45699.50685934028</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>schmitt</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>hschmitt@etu.isara.fr</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
       </c>
       <c r="D4" s="2">
-        <v>45699.508444548614</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
+        <v>45699.50844454861</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>schmitt</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>hschmitt</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>APPLICATIONNN</t>
+        </is>
       </c>
       <c r="D5" s="2">
-        <v>45699.517257407409</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
+        <v>45699.51725740741</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>hdhdhd</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>jhfhhfjdhdf</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>jhhfhehe</t>
+        </is>
       </c>
       <c r="D6" s="2">
-        <v>45699.521162000528</v>
+        <v>45699.52116200232</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sanchez</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>marie</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>cc</t>
+        </is>
+      </c>
+      <c r="D7" s="2">
+        <v>45699.52523977831</v>
       </c>
     </row>
   </sheetData>

</xml_diff>